<commit_message>
180213 / updated source
</commit_message>
<xml_diff>
--- a/doc/20180210_패키지별_CNN_실험결과.xlsx
+++ b/doc/20180210_패키지별_CNN_실험결과.xlsx
@@ -5,7 +5,7 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working_board\SPPNet_PyTorch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working_board\SPPNet_PyTorch\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>step</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -150,11 +150,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>malware</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>malware</t>
+    <t>tensorflow</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -162,7 +162,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="182" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,8 +189,32 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +236,16 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -319,29 +356,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1">
       <alignment vertical="center"/>
@@ -356,22 +396,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -380,12 +405,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -397,14 +431,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="4" fillId="5" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="5" fillId="6" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
+    <cellStyle name="나쁨" xfId="3" builtinId="27"/>
+    <cellStyle name="백분율" xfId="2" builtinId="5"/>
+    <cellStyle name="보통" xfId="4" builtinId="28"/>
     <cellStyle name="좋음" xfId="1" builtinId="26"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -435,7 +490,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[20180210_PyTorch_CNN_실험결과.xlsx]Sheet2!피벗 테이블3</c:name>
+    <c:name>[20180210_패키지별_CNN_실험결과.xlsx]Sheet2!피벗 테이블3</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -1082,7 +1137,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[20180210_PyTorch_CNN_실험결과.xlsx]Sheet2!피벗 테이블3</c:name>
+    <c:name>[20180210_패키지별_CNN_실험결과.xlsx]Sheet2!피벗 테이블3</c:name>
     <c:fmtId val="2"/>
   </c:pivotSource>
   <c:chart>
@@ -1723,7 +1778,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[20180210_PyTorch_CNN_실험결과.xlsx]Sheet2!피벗 테이블3</c:name>
+    <c:name>[20180210_패키지별_CNN_실험결과.xlsx]Sheet2!피벗 테이블3</c:name>
     <c:fmtId val="5"/>
   </c:pivotSource>
   <c:chart>
@@ -2400,7 +2455,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[20180210_PyTorch_CNN_실험결과.xlsx]Sheet2!피벗 테이블3</c:name>
+    <c:name>[20180210_패키지별_CNN_실험결과.xlsx]Sheet2!피벗 테이블3</c:name>
     <c:fmtId val="6"/>
   </c:pivotSource>
   <c:chart>
@@ -6237,7 +6292,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
@@ -6248,222 +6303,222 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>8.6699999999999999E-2</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <v>0.83614219665527301</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>0.11119999999999999</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>0.91246894836425696</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="5">
         <v>0.18140000000000001</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <v>0.92373596191406204</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
+      <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="5">
         <v>0.14099999999999999</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <v>0.91485420227050696</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+      <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="5">
         <v>0.23069999999999999</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="5">
         <v>0.88475654602050702</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
+      <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="5">
         <v>0.2019</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="5">
         <v>0.92288856506347605</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
+      <c r="A10" s="4">
         <v>7</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="5">
         <v>0.31040000000000001</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="5">
         <v>0.92100547790527298</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
+      <c r="A11" s="4">
         <v>8</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <v>0.24149999999999999</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="5">
         <v>0.89850296020507803</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
+      <c r="A12" s="4">
         <v>9</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="5">
         <v>0.2016</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="5">
         <v>0.91673721313476497</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
+      <c r="A13" s="4">
         <v>10</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <v>0.1605</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="5">
         <v>0.89137870788574203</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="6">
+      <c r="A14" s="4">
         <v>11</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="5">
         <v>0.1123</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="5">
         <v>0.91262588500976505</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
+      <c r="A15" s="4">
         <v>12</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="5">
         <v>0.31019999999999998</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="5">
         <v>0.89483093261718705</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="6">
+      <c r="A16" s="4">
         <v>13</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="5">
         <v>0.2097</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="5">
         <v>0.88494491577148404</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="6">
+      <c r="A17" s="4">
         <v>14</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="5">
         <v>6.3E-2</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="5">
         <v>0.91309661865234304</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="6">
+      <c r="A18" s="4">
         <v>15</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="5">
         <v>0.28710000000000002</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="5">
         <v>0.89128456115722599</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="6">
+      <c r="A19" s="4">
         <v>16</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="5">
         <v>0.12820000000000001</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="5">
         <v>0.88409751892089805</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="6">
+      <c r="A20" s="4">
         <v>17</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="5">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="5">
         <v>0.92235504150390601</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="6">
+      <c r="A21" s="4">
         <v>18</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="5">
         <v>0.1074</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="5">
         <v>0.920064010620117</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="6">
+      <c r="A22" s="4">
         <v>19</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="5">
         <v>9.7100000000000006E-2</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="5">
         <v>0.88714179992675701</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="5">
         <v>3.2769000000000013</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="5">
         <v>17.132912063598624</v>
       </c>
     </row>
@@ -6476,682 +6531,958 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="9.75" customWidth="1"/>
+    <col min="5" max="5" width="8.625" customWidth="1"/>
+    <col min="6" max="6" width="8.125" customWidth="1"/>
     <col min="8" max="8" width="4.125" customWidth="1"/>
+    <col min="10" max="10" width="8.5" customWidth="1"/>
+    <col min="11" max="11" width="8" customWidth="1"/>
+    <col min="12" max="12" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.75" customWidth="1"/>
+    <col min="15" max="15" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="23">
         <v>8.6699999999999999E-2</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="23">
         <v>97.018200397491398</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="23">
         <v>253.72483944892801</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="23">
         <v>67.540526628494206</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="23">
         <v>2.5076508522033598</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>0.83614219665527301</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="23">
         <v>0.11119999999999999</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="23">
         <v>98.632594347000094</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="23">
         <v>249.032622337341</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="23">
         <v>69.9601535797119</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="23">
         <v>2.4856438636779701</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>0.91246894836425696</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="M4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="24">
         <v>0.18140000000000001</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="24">
         <v>101.06022477149899</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="24">
         <v>247.12512850761399</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="24">
         <v>68.658817052841101</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="24">
         <v>2.5066502094268799</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="8">
         <v>0.92373596191406204</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="23">
         <f>B22</f>
         <v>0.17246842105263163</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="22">
         <f>G22</f>
         <v>0.9017322138736118</v>
       </c>
+      <c r="M5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="23">
+        <f>B36</f>
+        <v>0.12080790000000001</v>
+      </c>
+      <c r="O5" s="1">
+        <f>G36</f>
+        <v>0.92895521451212948</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="23">
         <v>0.14099999999999999</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="23">
         <v>99.344779968261705</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="23">
         <v>249.21767067909201</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="23">
         <v>70.981419324874807</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="23">
         <v>2.5066502094268799</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>0.91485420227050696</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="23">
         <f>INDEX(B3:B21, MATCH(K6, G3:G21,0))</f>
         <v>0.18140000000000001</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6" s="8">
         <f>MAX(G3:G21)</f>
         <v>0.92373596191406204</v>
       </c>
+      <c r="M6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="23">
+        <f>INDEX(B26:B35,MATCH(O6,G26:G35))</f>
+        <v>8.7915400000000005E-2</v>
+      </c>
+      <c r="O6" s="8">
+        <f>MAX(G26:G35)</f>
+        <v>0.93936540815365699</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="23">
         <v>0.23069999999999999</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="23">
         <v>102.13550400733899</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="23">
         <v>249.42372441291801</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="23">
         <v>71.575573921203599</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="23">
         <v>2.4836440086364702</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>0.88475654602050702</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="23">
         <v>0.2019</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="23">
         <v>102.643636226654</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="23">
         <v>250.77307462692201</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="23">
         <v>70.605322122573796</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="23">
         <v>2.5016493797302202</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>0.92288856506347605</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="23">
         <v>0.31040000000000001</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="23">
         <v>101.379307508468</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="23">
         <v>248.86157822608899</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="23">
         <v>72.3777818679809</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="23">
         <v>2.4836444854736301</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>0.92100547790527298</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="23">
         <v>0.24149999999999999</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="23">
         <v>103.59288191795299</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="23">
         <v>251.79634070396401</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="23">
         <v>70.7053475379943</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="23">
         <v>2.4896454811096098</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <v>0.89850296020507803</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="23">
         <v>0.2016</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="23">
         <v>102.09249305725</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="23">
         <v>253.61281204223599</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="23">
         <v>69.705088376998901</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="23">
         <v>2.4686403274536102</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>0.91673721313476497</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="23">
         <v>0.1605</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="23">
         <v>101.240271568298</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="23">
         <v>253.670826435089</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="23">
         <v>70.985420703887897</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="23">
         <v>2.4636385440826398</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <v>0.89137870788574203</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
         <v>11</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="23">
         <v>0.1123</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="23">
         <v>102.42757964134201</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="23">
         <v>250.99213385581899</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="23">
         <v>71.489551067352295</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="23">
         <v>2.4776437282562198</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <v>0.91262588500976505</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="10">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
         <v>12</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="23">
         <v>0.31019999999999998</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="23">
         <v>104.337075233459</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="23">
         <v>251.64030051231299</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="23">
         <v>69.612063884735093</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="23">
         <v>2.4886455535888601</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <v>0.89483093261718705</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="10">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
         <v>13</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="23">
         <v>0.2097</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="23">
         <v>102.43358135223301</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="23">
         <v>249.565761566162</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="23">
         <v>71.444539785385103</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="23">
         <v>2.4546368122100799</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <v>0.88494491577148404</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="10">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
         <v>14</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="23">
         <v>6.3E-2</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="23">
         <v>104.591140985488</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="23">
         <v>250.72706294059699</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="23">
         <v>72.8899147510528</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="23">
         <v>2.4726419448852499</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="1">
         <v>0.91309661865234304</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="10">
+      <c r="A17" s="7">
         <v>15</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="23">
         <v>0.28710000000000002</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="23">
         <v>106.27557849884001</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="23">
         <v>251.01313781738199</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="23">
         <v>71.868649721145601</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="23">
         <v>2.4616389274597101</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="1">
         <v>0.89128456115722599</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="10">
+      <c r="A18" s="7">
         <v>16</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="23">
         <v>0.12820000000000001</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="23">
         <v>103.00072813033999</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="23">
         <v>252.29747009277301</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="23">
         <v>73.893174648284898</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="23">
         <v>2.4396333694457999</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="1">
         <v>0.88409751892089805</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
+      <c r="A19" s="7">
         <v>17</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="23">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="23">
         <v>105.413354873657</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="23">
         <v>250.605031728744</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="23">
         <v>75.121494054794297</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="23">
         <v>2.4496357440948402</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="1">
         <v>0.92235504150390601</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="10">
+      <c r="A20" s="7">
         <v>18</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="23">
         <v>0.1074</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="23">
         <v>108.184073448181</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="23">
         <v>250.35496664047201</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="23">
         <v>73.3410320281982</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="23">
         <v>2.4536366462707502</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="1">
         <v>0.920064010620117</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
+      <c r="A21" s="7">
         <v>19</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="23">
         <v>9.7100000000000006E-2</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="23">
         <v>107.05678105354301</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="23">
         <v>250.55001807212801</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="23">
         <v>74.307282209396305</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="23">
         <v>2.4496355056762602</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="1">
         <v>0.88714179992675701</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="23">
         <f>AVERAGE(B3:B21)</f>
         <v>0.17246842105263163</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="25">
         <f>AVERAGE(C3:C21)</f>
         <v>102.782094051963</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="26">
         <f t="shared" ref="D22:G22" si="0">AVERAGE(D3:D21)</f>
         <v>250.78865792876758</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="25">
         <f t="shared" si="0"/>
         <v>71.424376487731905</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="26">
         <f t="shared" si="0"/>
         <v>2.4760634522688973</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="21">
         <f t="shared" si="0"/>
         <v>0.9017322138736118</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="8" t="s">
+      <c r="B24" s="20"/>
+      <c r="C24" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8" t="s">
+      <c r="D24" s="15"/>
+      <c r="E24" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="I24" s="16" t="s">
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="I24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J24" s="9" t="s">
+      <c r="J24" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K24" s="9" t="s">
+      <c r="K24" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L24" s="9" t="s">
+      <c r="L24" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I25" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J25" s="17" t="s">
+      <c r="I25" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J25" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="K25" s="17" t="s">
+      <c r="K25" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="L25" s="20"/>
+      <c r="L25" s="16"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="10">
+      <c r="A26" s="7">
         <v>1</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4">
-        <v>796.45399999999995</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4">
-        <v>61.18</v>
-      </c>
-      <c r="G26" s="14">
-        <v>0.93200000000000005</v>
-      </c>
-      <c r="I26" s="8"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="21"/>
+      <c r="B26" s="23">
+        <v>6.4680399999999999E-2</v>
+      </c>
+      <c r="C26" s="23">
+        <v>31.506767034530601</v>
+      </c>
+      <c r="D26" s="23">
+        <v>1089.69831967353</v>
+      </c>
+      <c r="E26" s="23">
+        <v>21.973689556121801</v>
+      </c>
+      <c r="F26" s="23">
+        <v>66.9273295402526</v>
+      </c>
+      <c r="G26" s="22">
+        <v>0.93497159715029898</v>
+      </c>
+      <c r="I26" s="15"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="17"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I27" s="8" t="s">
+      <c r="A27" s="7">
+        <v>2</v>
+      </c>
+      <c r="B27" s="23">
+        <v>0.102479</v>
+      </c>
+      <c r="C27" s="23">
+        <v>31.616186141967699</v>
+      </c>
+      <c r="D27" s="23">
+        <v>1091.0234959125501</v>
+      </c>
+      <c r="E27" s="23">
+        <v>22.2597637176513</v>
+      </c>
+      <c r="F27" s="23">
+        <v>70.265193462371798</v>
+      </c>
+      <c r="G27" s="22">
+        <v>0.93767065248093395</v>
+      </c>
+      <c r="I27" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="J27" s="17" t="s">
+      <c r="J27" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="K27" s="17" t="s">
+      <c r="K27" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="L27" s="21"/>
+      <c r="L27" s="17"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I28" s="8"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="22"/>
+      <c r="A28" s="7">
+        <v>3</v>
+      </c>
+      <c r="B28" s="23">
+        <v>8.92424E-2</v>
+      </c>
+      <c r="C28" s="23">
+        <v>32.147323131561201</v>
+      </c>
+      <c r="D28" s="23">
+        <v>1086.1612365245801</v>
+      </c>
+      <c r="E28" s="23">
+        <v>22.970948219299299</v>
+      </c>
+      <c r="F28" s="23">
+        <v>69.726053953170705</v>
+      </c>
+      <c r="G28" s="22">
+        <v>0.93399868185669899</v>
+      </c>
+      <c r="I28" s="15"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="18"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I29" s="9" t="s">
+      <c r="A29" s="7">
+        <v>4</v>
+      </c>
+      <c r="B29" s="23">
+        <v>0.10838200000000001</v>
+      </c>
+      <c r="C29" s="23">
+        <v>33.145582675933802</v>
+      </c>
+      <c r="D29" s="23">
+        <v>1077.9100999832101</v>
+      </c>
+      <c r="E29" s="23">
+        <v>23.248019933700501</v>
+      </c>
+      <c r="F29" s="23">
+        <v>73.596055746078406</v>
+      </c>
+      <c r="G29" s="22">
+        <v>0.93180177635501904</v>
+      </c>
+      <c r="I29" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J29" s="23"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="19">
+      <c r="J29" s="11"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="10">
         <v>76846</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>5</v>
+      </c>
+      <c r="B30" s="23">
+        <v>4.4273800000000002E-2</v>
+      </c>
+      <c r="C30" s="23">
+        <v>33.462663650512603</v>
+      </c>
+      <c r="D30" s="23">
+        <v>1090.02623772621</v>
+      </c>
+      <c r="E30" s="23">
+        <v>23.935197353363002</v>
+      </c>
+      <c r="F30" s="23">
+        <v>67.4724698066711</v>
+      </c>
+      <c r="G30" s="22">
+        <v>0.936446662272855</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="7">
+        <v>6</v>
+      </c>
+      <c r="B31" s="23">
+        <v>0.32118600000000003</v>
+      </c>
+      <c r="C31" s="23">
+        <v>34.792008399963301</v>
+      </c>
+      <c r="D31" s="23">
+        <v>1097.77524495124</v>
+      </c>
+      <c r="E31" s="23">
+        <v>24.325298309326101</v>
+      </c>
+      <c r="F31" s="23">
+        <v>76.399781942367497</v>
+      </c>
+      <c r="G31" s="22">
+        <v>0.91774158114427395</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
+        <v>7</v>
+      </c>
+      <c r="B32" s="23">
+        <v>0.15834000000000001</v>
+      </c>
+      <c r="C32" s="23">
+        <v>35.780264377593902</v>
+      </c>
+      <c r="D32" s="23">
+        <v>1072.24063277244</v>
+      </c>
+      <c r="E32" s="23">
+        <v>25.058488607406598</v>
+      </c>
+      <c r="F32" s="23">
+        <v>60.722722053527797</v>
+      </c>
+      <c r="G32" s="22">
+        <v>0.929196874117314</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
+        <v>8</v>
+      </c>
+      <c r="B33" s="24">
+        <v>8.7915400000000005E-2</v>
+      </c>
+      <c r="C33" s="24">
+        <v>36.8685462474823</v>
+      </c>
+      <c r="D33" s="24">
+        <v>1087.1855030059801</v>
+      </c>
+      <c r="E33" s="24">
+        <v>25.1555128097534</v>
+      </c>
+      <c r="F33" s="24">
+        <v>66.107116222381507</v>
+      </c>
+      <c r="G33" s="8">
+        <v>0.93936540815365699</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
+        <v>9</v>
+      </c>
+      <c r="B34" s="23">
+        <v>0.147174</v>
+      </c>
+      <c r="C34" s="23">
+        <v>37.286653757095301</v>
+      </c>
+      <c r="D34" s="23">
+        <v>1063.42458319664</v>
+      </c>
+      <c r="E34" s="23">
+        <v>25.636637926101599</v>
+      </c>
+      <c r="F34" s="23">
+        <v>69.620025634765597</v>
+      </c>
+      <c r="G34" s="22">
+        <v>0.898816809465524</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="7">
+        <v>10</v>
+      </c>
+      <c r="B35" s="23">
+        <v>8.4405999999999995E-2</v>
+      </c>
+      <c r="C35" s="23">
+        <v>37.676755666732703</v>
+      </c>
+      <c r="D35" s="23">
+        <v>1086.35328650474</v>
+      </c>
+      <c r="E35" s="23">
+        <v>26.174776792526199</v>
+      </c>
+      <c r="F35" s="23">
+        <v>70.170168399810706</v>
+      </c>
+      <c r="G35" s="22">
+        <v>0.92954210212472099</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="23">
+        <f>AVERAGE(B26:B35)</f>
+        <v>0.12080790000000001</v>
+      </c>
+      <c r="C36" s="25">
+        <f t="shared" ref="C36:G36" si="1">AVERAGE(C26:C35)</f>
+        <v>34.428275108337346</v>
+      </c>
+      <c r="D36" s="26">
+        <f t="shared" si="1"/>
+        <v>1084.179864025112</v>
+      </c>
+      <c r="E36" s="25">
+        <f t="shared" si="1"/>
+        <v>24.073833322524976</v>
+      </c>
+      <c r="F36" s="26">
+        <f t="shared" si="1"/>
+        <v>69.100691676139775</v>
+      </c>
+      <c r="G36" s="21">
+        <f t="shared" si="1"/>
+        <v>0.92895521451212948</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="L25:L28"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:G1"/>
     <mergeCell ref="J29:K29"/>
     <mergeCell ref="J27:J28"/>
     <mergeCell ref="K27:K28"/>
     <mergeCell ref="I25:I26"/>
     <mergeCell ref="I27:I28"/>
-    <mergeCell ref="L25:L28"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:G24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>